<commit_message>
new nimbus R6 and date
</commit_message>
<xml_diff>
--- a/FlightGUIwithTestIterationLoop_1stDecFlights/Default.xlsx
+++ b/FlightGUIwithTestIterationLoop_1stDecFlights/Default.xlsx
@@ -246,13 +246,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="7" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="7" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -554,13 +554,13 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1484375" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="2" width="9.1484375" style="4" customWidth="1"/>
-    <col min="3" max="3" width="9.41796875" style="3" customWidth="1"/>
+    <col min="1" max="2" width="9.1484375" style="5" customWidth="1"/>
+    <col min="3" max="3" width="9.41796875" style="4" customWidth="1"/>
     <col min="4" max="16384" width="9.1484375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -582,7 +582,7 @@
       <c s="2" t="s">
         <v>0</v>
       </c>
-      <c s="5">
+      <c s="3">
         <v>222</v>
       </c>
     </row>
@@ -593,7 +593,7 @@
       <c s="2" t="s">
         <v>3</v>
       </c>
-      <c s="5">
+      <c s="3">
         <v>214.94</v>
       </c>
     </row>
@@ -604,7 +604,7 @@
       <c s="2" t="s">
         <v>7</v>
       </c>
-      <c s="5">
+      <c s="3">
         <v>337.60000000000002</v>
       </c>
     </row>

</xml_diff>

<commit_message>
new date and costs used gitbash couldnt do this in UFT
</commit_message>
<xml_diff>
--- a/FlightGUIwithTestIterationLoop_1stDecFlights/Default.xlsx
+++ b/FlightGUIwithTestIterationLoop_1stDecFlights/Default.xlsx
@@ -246,10 +246,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="7" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="7" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
@@ -560,52 +560,52 @@
   <sheetFormatPr defaultColWidth="9.1484375" defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="2" width="9.1484375" style="5" customWidth="1"/>
-    <col min="3" max="3" width="9.41796875" style="4" customWidth="1"/>
+    <col min="3" max="3" width="9.41796875" style="3" customWidth="1"/>
     <col min="4" max="16384" width="9.1484375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row ht="12.75" customHeight="1" customFormat="1">
-      <c t="s">
+    <row r="1" ht="12.75" customHeight="1" customFormat="1">
+      <c r="A1" t="s">
         <v>4</v>
       </c>
-      <c t="s">
+      <c r="B1" t="s">
         <v>5</v>
       </c>
-      <c t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row s="1" customFormat="1">
-      <c s="2" t="s">
+    <row r="2" s="1" customFormat="1">
+      <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
-      <c s="2" t="s">
+      <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
-      <c s="3">
-        <v>222</v>
+      <c r="C2" s="4">
+        <v>356.94</v>
       </c>
     </row>
-    <row s="1" customFormat="1">
-      <c s="2" t="s">
+    <row r="3" s="1" customFormat="1">
+      <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
-      <c s="2" t="s">
+      <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
-      <c s="3">
-        <v>214.94</v>
+      <c r="C3" s="4">
+        <v>336.39999999999998</v>
       </c>
     </row>
-    <row s="1" customFormat="1">
-      <c s="2" t="s">
+    <row r="4" s="1" customFormat="1">
+      <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
-      <c s="2" t="s">
+      <c r="B4" s="2" t="s">
         <v>7</v>
       </c>
-      <c s="3">
-        <v>337.60000000000002</v>
+      <c r="C4" s="4">
+        <v>350.94</v>
       </c>
     </row>
   </sheetData>
@@ -631,7 +631,7 @@
     <col min="1" max="16384" width="9.1484375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row ht="12.75" customHeight="1" customFormat="1"/>
+    <row r="1" ht="12.75" customHeight="1" customFormat="1"/>
   </sheetData>
   <printOptions gridLines="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -655,7 +655,7 @@
     <col min="1" max="16384" width="9.1484375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row ht="12.75" customHeight="1" customFormat="1"/>
+    <row r="1" ht="12.75" customHeight="1" customFormat="1"/>
   </sheetData>
   <printOptions gridLines="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -679,7 +679,7 @@
     <col min="1" max="16384" width="9.1484375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row ht="12.75" customHeight="1" customFormat="1"/>
+    <row r="1" ht="12.75" customHeight="1" customFormat="1"/>
   </sheetData>
   <printOptions gridLines="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
new dates and costs
</commit_message>
<xml_diff>
--- a/FlightGUIwithTestIterationLoop_1stDecFlights/Default.xlsx
+++ b/FlightGUIwithTestIterationLoop_1stDecFlights/Default.xlsx
@@ -554,7 +554,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1484375" defaultRowHeight="13.5"/>
@@ -583,7 +583,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="4">
-        <v>356.94</v>
+        <v>246</v>
       </c>
     </row>
     <row r="3" s="1" customFormat="1">
@@ -594,7 +594,7 @@
         <v>3</v>
       </c>
       <c r="C3" s="4">
-        <v>336.39999999999998</v>
+        <v>278.94</v>
       </c>
     </row>
     <row r="4" s="1" customFormat="1">
@@ -605,7 +605,7 @@
         <v>7</v>
       </c>
       <c r="C4" s="4">
-        <v>350.94</v>
+        <v>385.60000000000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>